<commit_message>
first attempt at RadarEffect()
</commit_message>
<xml_diff>
--- a/PartsListESP32Clock.xlsx
+++ b/PartsListESP32Clock.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{214DB1BC-DC82-448F-9BD0-AF3738B2B644}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2398B72-A5B7-45DE-B660-E9647F06D670}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="915" yWindow="3450" windowWidth="35880" windowHeight="10545" activeTab="1" xr2:uid="{41B2ED1C-8C08-4B2A-A527-B1C849EDAEC9}"/>
+    <workbookView xWindow="915" yWindow="3450" windowWidth="35880" windowHeight="10545" activeTab="2" xr2:uid="{41B2ED1C-8C08-4B2A-A527-B1C849EDAEC9}"/>
   </bookViews>
   <sheets>
     <sheet name="PartsList" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="67">
   <si>
     <t>https://smile.amazon.com/gp/product/B08DQQ8CBP/</t>
   </si>
@@ -126,12 +126,6 @@
     <t>const uint16_t  leds_per_ring[NUM_RINGS_PER_DISK]  = { MAX_LEDS_PER_RING, 48, 40, 32, 24, 16, 12, 8, MIN_LEDS_PER_RING }; // MAX_LEDS_PER_RING = 60</t>
   </si>
   <si>
-    <t>const uint8_t   start_per_ring[NUM_RINGS_PER_DISK] = {  0, 60, 108, 148, 180, 204, 220, 232, 240 }; // which LED index is the start of each ring</t>
-  </si>
-  <si>
-    <t>const uint8_t  radar_adv_per_LED_per_ring[NUM_RINGS_PER_DISK] = { , , , , , , , , };</t>
-  </si>
-  <si>
     <t>const uint16_t  leds_per_ringqrtr[NUM_RINGS_PER_DISK]  = { 15, 12, 10, 8, 6, 4, 3, 2, 1 };</t>
   </si>
   <si>
@@ -229,6 +223,9 @@
   </si>
   <si>
     <t xml:space="preserve"> { 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, </t>
+  </si>
+  <si>
+    <t>const uint16_t   start_per_ring[NUM_RINGS_PER_DISK] = {  0, 60, 108, 148, 180, 204, 220, 232, 240 }; // which LED index is the start of each ring</t>
   </si>
 </sst>
 </file>
@@ -920,7 +917,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9251FEAC-53B0-4F8C-BA59-E6CC86FBF419}">
   <dimension ref="A1:N26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
@@ -1365,8 +1362,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{533DE995-FBF8-4304-AE97-4EE9DF4E65CB}">
   <dimension ref="A1:AB94"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="S20" sqref="S20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1376,22 +1373,22 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
@@ -1401,47 +1398,42 @@
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>34</v>
+        <v>66</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="17" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="18" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="19" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="20" spans="1:28" x14ac:dyDescent="0.25">
       <c r="H20" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="I20">
         <v>0</v>
@@ -1503,10 +1495,10 @@
     </row>
     <row r="21" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B21" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D21" s="5" t="s">
         <v>21</v>
@@ -1556,34 +1548,34 @@
         <v>60</v>
       </c>
       <c r="I22" t="s">
+        <v>45</v>
+      </c>
+      <c r="J22" t="s">
+        <v>46</v>
+      </c>
+      <c r="K22" t="s">
         <v>47</v>
       </c>
-      <c r="J22" t="s">
+      <c r="L22" t="s">
         <v>48</v>
       </c>
-      <c r="K22" t="s">
+      <c r="M22" t="s">
         <v>49</v>
       </c>
-      <c r="L22" t="s">
+      <c r="N22" t="s">
         <v>50</v>
       </c>
-      <c r="M22" t="s">
+      <c r="O22" t="s">
         <v>51</v>
       </c>
-      <c r="N22" t="s">
+      <c r="P22" t="s">
         <v>52</v>
       </c>
-      <c r="O22" t="s">
+      <c r="Q22" t="s">
         <v>53</v>
       </c>
-      <c r="P22" t="s">
-        <v>54</v>
-      </c>
-      <c r="Q22" t="s">
+      <c r="S22" t="s">
         <v>55</v>
-      </c>
-      <c r="S22" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="23" spans="1:28" x14ac:dyDescent="0.25">
@@ -6058,7 +6050,7 @@
     </row>
     <row r="83" spans="9:28" x14ac:dyDescent="0.25">
       <c r="S83" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="T83" t="str">
         <f t="shared" si="4"/>
@@ -6099,47 +6091,47 @@
     </row>
     <row r="86" spans="9:28" x14ac:dyDescent="0.25">
       <c r="T86" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="87" spans="9:28" x14ac:dyDescent="0.25">
       <c r="T87" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="88" spans="9:28" x14ac:dyDescent="0.25">
       <c r="T88" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="89" spans="9:28" x14ac:dyDescent="0.25">
       <c r="T89" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="90" spans="9:28" x14ac:dyDescent="0.25">
       <c r="T90" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="91" spans="9:28" x14ac:dyDescent="0.25">
       <c r="T91" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="92" spans="9:28" x14ac:dyDescent="0.25">
       <c r="T92" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="93" spans="9:28" x14ac:dyDescent="0.25">
       <c r="T93" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="94" spans="9:28" x14ac:dyDescent="0.25">
       <c r="T94" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix memcpy bug, add debug, add some parts
</commit_message>
<xml_diff>
--- a/PartsListESP32Clock.xlsx
+++ b/PartsListESP32Clock.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{594C8D87-BF09-47F1-AA94-6AE6AB58D821}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7932849-55D0-47D8-8BCC-7AD216F9B558}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" activeTab="2" xr2:uid="{41B2ED1C-8C08-4B2A-A527-B1C849EDAEC9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{41B2ED1C-8C08-4B2A-A527-B1C849EDAEC9}"/>
   </bookViews>
   <sheets>
     <sheet name="PartsList" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="78">
   <si>
     <t>https://smile.amazon.com/gp/product/B08DQQ8CBP/</t>
   </si>
@@ -241,6 +241,24 @@
   </si>
   <si>
     <t xml:space="preserve"> { 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0 },</t>
+  </si>
+  <si>
+    <t>10K Ohm resistor, 1/4 watt</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/stackpole-electronics-inc/CF14JT10K0/1741265</t>
+  </si>
+  <si>
+    <t>0.1 uF electrolytic capacitor</t>
+  </si>
+  <si>
+    <t>100 uF electrolytic capacitor</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/w%C3%BCrth-elektronik/860010672001/5728608</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/panasonic-electronic-components/ECA-2AM101/245067</t>
   </si>
 </sst>
 </file>
@@ -673,10 +691,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B29A9E47-469B-441B-BC4B-4F95D35E1C9E}">
-  <dimension ref="A1:K8"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9:G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -814,7 +832,7 @@
         <v>2</v>
       </c>
       <c r="G5" t="str">
-        <f t="shared" si="1"/>
+        <f>"| "&amp;A5&amp;" | $"&amp;TEXT(B5,"0.00")&amp;" | $"&amp;TEXT(C5,"0.00")&amp;" | "&amp;D5&amp;" | "&amp;E5&amp;" |"</f>
         <v>| 0 | $6.00 | $0.00 | ESP32 ESP-32S CP2102 NodeMCU-32S ESP-WROOM-32 WiFi | https://smile.amazon.com/DORHEA-Development-Microcontroller-NodeMCU-32S-ESP-WROOM-32/dp/B086MJGFVV/ |</v>
       </c>
       <c r="J5" s="1">
@@ -901,13 +919,100 @@
         <v>18</v>
       </c>
       <c r="G8" t="str">
-        <f t="shared" ref="G8" si="4">"| "&amp;A8&amp;" | $"&amp;TEXT(B8,"0.00")&amp;" | $"&amp;TEXT(C8,"0.00")&amp;" | "&amp;D8&amp;" | "&amp;E8&amp;" |"</f>
+        <f t="shared" ref="G8:G11" si="4">"| "&amp;A8&amp;" | $"&amp;TEXT(B8,"0.00")&amp;" | $"&amp;TEXT(C8,"0.00")&amp;" | "&amp;D8&amp;" | "&amp;E8&amp;" |"</f>
         <v>| 1 | $0.10 | $0.10 | 220 Ohm resistor, 1/4 watt (optional) | https://www.digikey.com/en/products/detail/stackpole-electronics-inc/CF14JT220R/1741346 |</v>
       </c>
       <c r="J8" s="1">
         <v>0.1</v>
       </c>
       <c r="K8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9" s="1">
+        <f t="shared" ref="B9" si="5">J9/K9</f>
+        <v>0.1</v>
+      </c>
+      <c r="C9" s="1">
+        <f t="shared" ref="C9" si="6">A9*B9</f>
+        <v>0.1</v>
+      </c>
+      <c r="D9" t="s">
+        <v>72</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="G9" t="str">
+        <f t="shared" si="4"/>
+        <v>| 1 | $0.10 | $0.10 | 10K Ohm resistor, 1/4 watt | https://www.digikey.com/en/products/detail/stackpole-electronics-inc/CF14JT10K0/1741265 |</v>
+      </c>
+      <c r="J9" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="K9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="B10" s="1">
+        <f t="shared" ref="B10:B11" si="7">J10/K10</f>
+        <v>0.1</v>
+      </c>
+      <c r="C10" s="1">
+        <f t="shared" ref="C10" si="8">A10*B10</f>
+        <v>0.1</v>
+      </c>
+      <c r="D10" t="s">
+        <v>74</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="G10" t="str">
+        <f t="shared" si="4"/>
+        <v>| 1 | $0.10 | $0.10 | 0.1 uF electrolytic capacitor | https://www.digikey.com/en/products/detail/w%C3%BCrth-elektronik/860010672001/5728608 |</v>
+      </c>
+      <c r="J10" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="K10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11" s="1">
+        <f t="shared" ref="B11" si="9">J11/K11</f>
+        <v>0.53</v>
+      </c>
+      <c r="C11" s="1">
+        <f t="shared" ref="C11" si="10">A11*B11</f>
+        <v>0.53</v>
+      </c>
+      <c r="D11" t="s">
+        <v>75</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="G11" t="str">
+        <f t="shared" si="4"/>
+        <v>| 1 | $0.53 | $0.53 | 100 uF electrolytic capacitor | https://www.digikey.com/en/products/detail/panasonic-electronic-components/ECA-2AM101/245067 |</v>
+      </c>
+      <c r="J11" s="1">
+        <v>0.53</v>
+      </c>
+      <c r="K11">
         <v>1</v>
       </c>
     </row>
@@ -922,9 +1027,12 @@
     <hyperlink ref="E6" r:id="rId4" xr:uid="{E3BAB0B9-CE51-4BA0-89FD-4B596A712210}"/>
     <hyperlink ref="E7" r:id="rId5" xr:uid="{779703E2-59B3-475E-9C2F-63D23BB576F3}"/>
     <hyperlink ref="E8" r:id="rId6" xr:uid="{1C8C588A-E60D-43AB-AD56-45C43B9F934B}"/>
+    <hyperlink ref="E9" r:id="rId7" xr:uid="{CFD1EBA0-D500-4DFE-8134-A59E85C63B37}"/>
+    <hyperlink ref="E10" r:id="rId8" xr:uid="{BBD8A739-5643-4B84-95CF-8ABC696BDA3D}"/>
+    <hyperlink ref="E11" r:id="rId9" xr:uid="{9D4426D0-FEDC-42AE-984A-B5D2B499A2ED}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId7"/>
+  <pageSetup orientation="portrait" r:id="rId10"/>
 </worksheet>
 </file>
 
@@ -1377,8 +1485,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{533DE995-FBF8-4304-AE97-4EE9DF4E65CB}">
   <dimension ref="A1:AC169"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A136" workbookViewId="0">
-      <selection activeCell="T161" sqref="T161:T169"/>
+    <sheetView topLeftCell="A136" workbookViewId="0">
+      <selection activeCell="L171" sqref="L171"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>